<commit_message>
???????? ????????? ??????. ????????? XML ??????, ????? ???????? ??????.
</commit_message>
<xml_diff>
--- a/reports/ags-1.xlsx
+++ b/reports/ags-1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="14805" windowHeight="8070"/>
@@ -15,12 +15,12 @@
     <definedName name="spec_f">Лист1!$A$53:$T$53</definedName>
     <definedName name="spec_s">Лист1!$A$54:$T$54</definedName>
   </definedNames>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
   <si>
     <t>ФЕДЕРАЛЬНОЕ СТАТИСТИЧЕСКОЕ НАБЛЮДЕНИЕ</t>
   </si>
@@ -287,37 +287,10 @@
     <t>${others}</t>
   </si>
   <si>
-    <t>${beg_ed}</t>
-  </si>
-  <si>
-    <t>${osn_ed}</t>
-  </si>
-  <si>
-    <t>${mid_ed}</t>
-  </si>
-  <si>
-    <t>${beg_pr}</t>
-  </si>
-  <si>
-    <t>${mid_pr}</t>
-  </si>
-  <si>
-    <t>${up_pr}</t>
-  </si>
-  <si>
     <t>${dates}</t>
   </si>
   <si>
     <t>${doca}</t>
-  </si>
-  <si>
-    <t>${all_humans1}</t>
-  </si>
-  <si>
-    <t>${all_humans2}</t>
-  </si>
-  <si>
-    <t>${all_humans3}</t>
   </si>
   <si>
     <t>${beg_ed1}</t>
@@ -1602,7 +1575,9 @@
   </sheetPr>
   <dimension ref="B1:T89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1727,7 +1702,7 @@
     <row r="12" spans="3:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="E13" s="68" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F13" s="69"/>
       <c r="G13" s="69"/>
@@ -2057,11 +2032,11 @@
     </row>
     <row r="35" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="124" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C35" s="125"/>
       <c r="D35" s="124" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E35" s="125"/>
       <c r="F35" s="125">
@@ -2121,7 +2096,7 @@
       </c>
       <c r="F41" s="133"/>
       <c r="G41" s="100" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="H41" s="101"/>
       <c r="I41" s="101"/>
@@ -2737,33 +2712,39 @@
       <c r="F66" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="G66" s="20" t="e">
-        <f>S52</f>
-        <v>#VALUE!</v>
+      <c r="G66" s="20">
+        <f>SUM(G69:H74)</f>
+        <v>0</v>
       </c>
       <c r="H66" s="20"/>
-      <c r="I66" s="20" t="s">
-        <v>70</v>
+      <c r="I66" s="20">
+        <f>SUM(I69:J74)</f>
+        <v>0</v>
       </c>
       <c r="J66" s="20"/>
-      <c r="K66" s="20" t="s">
-        <v>71</v>
+      <c r="K66" s="20">
+        <f>SUM(K69:L74)</f>
+        <v>0</v>
       </c>
       <c r="L66" s="20"/>
-      <c r="M66" s="20" t="s">
-        <v>72</v>
+      <c r="M66" s="20">
+        <f>SUM(M69:N74)</f>
+        <v>0</v>
       </c>
       <c r="N66" s="20"/>
-      <c r="O66" s="20" t="s">
-        <v>73</v>
+      <c r="O66" s="20">
+        <f>SUM(O69:P74)</f>
+        <v>0</v>
       </c>
       <c r="P66" s="20"/>
-      <c r="Q66" s="20" t="s">
-        <v>74</v>
+      <c r="Q66" s="20">
+        <f>SUM(Q69:R74)</f>
+        <v>0</v>
       </c>
       <c r="R66" s="20"/>
-      <c r="S66" s="20" t="s">
-        <v>75</v>
+      <c r="S66" s="20">
+        <f>SUM(S69:T74)</f>
+        <v>0</v>
       </c>
       <c r="T66" s="20"/>
     </row>
@@ -2819,32 +2800,33 @@
       <c r="F69" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="G69" s="25" t="s">
-        <v>78</v>
+      <c r="G69" s="25">
+        <f>SUM(I69:T70)</f>
+        <v>0</v>
       </c>
       <c r="H69" s="26"/>
       <c r="I69" s="20" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="J69" s="20"/>
       <c r="K69" s="20" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="L69" s="20"/>
       <c r="M69" s="20" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="N69" s="20"/>
       <c r="O69" s="20" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="P69" s="20"/>
       <c r="Q69" s="20" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="R69" s="20"/>
       <c r="S69" s="20" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="T69" s="20"/>
     </row>
@@ -2879,32 +2861,33 @@
       <c r="F71" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="G71" s="25" t="s">
-        <v>79</v>
+      <c r="G71" s="25">
+        <f>SUM(I71:T72)</f>
+        <v>0</v>
       </c>
       <c r="H71" s="26"/>
       <c r="I71" s="20" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="J71" s="20"/>
       <c r="K71" s="20" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="L71" s="20"/>
       <c r="M71" s="20" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="N71" s="20"/>
       <c r="O71" s="20" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="P71" s="20"/>
       <c r="Q71" s="20" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="R71" s="20"/>
       <c r="S71" s="20" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="T71" s="20"/>
     </row>
@@ -2939,32 +2922,33 @@
       <c r="F73" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G73" s="25" t="s">
-        <v>80</v>
+      <c r="G73" s="25">
+        <f>SUM(I73:T74)</f>
+        <v>0</v>
       </c>
       <c r="H73" s="26"/>
       <c r="I73" s="20" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="J73" s="20"/>
       <c r="K73" s="20" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="L73" s="20"/>
       <c r="M73" s="20" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="N73" s="20"/>
       <c r="O73" s="20" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="P73" s="20"/>
       <c r="Q73" s="20" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="R73" s="20"/>
       <c r="S73" s="20" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="T73" s="20"/>
     </row>
@@ -3152,7 +3136,7 @@
       <c r="G87" s="16"/>
       <c r="H87" s="11"/>
       <c r="I87" s="17" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="J87" s="17"/>
       <c r="K87" s="17"/>

</xml_diff>